<commit_message>
Aula 13: for paralelo
</commit_message>
<xml_diff>
--- a/plano-de-aulas-t1.xlsx
+++ b/plano-de-aulas-t1.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Copy of Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Copy of Sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>Data</t>
   </si>
@@ -192,6 +193,18 @@
   </si>
   <si>
     <t xml:space="preserve">Prova Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisão da prova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introdução a paralelismo - teoria e experimentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula expositiva de 30 minutos; Aceleração de operações usando tarefas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula expositiva de 30 minutos; Aceleração usando paralelismo de dados.</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução ao curso; Princípios de C++</t>
@@ -2323,6 +2336,1249 @@
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
+      <selection activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" style="1" width="14.375"/>
+    <col customWidth="1" min="2" max="2" style="1" width="11.625"/>
+    <col customWidth="1" min="3" max="3" style="1" width="26.440000000000001"/>
+    <col customWidth="1" min="4" max="4" style="1" width="16.670000000000002"/>
+    <col customWidth="1" min="5" max="5" style="1" width="15.789999999999999"/>
+    <col customWidth="1" min="6" max="6" style="1" width="24.109999999999999"/>
+    <col customWidth="1" min="7" max="27" style="1" width="11"/>
+    <col customWidth="1" min="28" max="1025" style="1" width="11.26"/>
+    <col min="1026" max="16384" style="1" width="9.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="29.399999999999999" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" ht="63.649999999999999" customHeight="1">
+      <c r="A2" s="5">
+        <v>44068</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+    </row>
+    <row r="3" ht="75.549999999999997" customHeight="1">
+      <c r="A3" s="5">
+        <v>44071</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+    </row>
+    <row r="4" ht="39.75" customHeight="1">
+      <c r="A4" s="5">
+        <f>A2+7</f>
+        <v>44075</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+    </row>
+    <row r="5" ht="39.75" customHeight="1">
+      <c r="A5" s="5">
+        <f>A3+7</f>
+        <v>44078</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+    </row>
+    <row r="6" ht="39.75" customHeight="1">
+      <c r="A6" s="5">
+        <f>A4+7</f>
+        <v>44082</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+    </row>
+    <row r="7" ht="39.75" customHeight="1">
+      <c r="A7" s="5">
+        <f>A5+7</f>
+        <v>44085</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+    </row>
+    <row r="8" ht="63.649999999999999" customHeight="1">
+      <c r="A8" s="5">
+        <f>A6+7</f>
+        <v>44089</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+    </row>
+    <row r="9" ht="51.700000000000003" customHeight="1">
+      <c r="A9" s="5">
+        <f>A7+7</f>
+        <v>44092</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+    </row>
+    <row r="10" ht="75.549999999999997" customHeight="1">
+      <c r="A10" s="5">
+        <f>A8+7</f>
+        <v>44096</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+    </row>
+    <row r="11" ht="51.700000000000003" customHeight="1">
+      <c r="A11" s="5">
+        <f>A9+7</f>
+        <v>44099</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+    </row>
+    <row r="12" ht="63.649999999999999" customHeight="1">
+      <c r="A12" s="5">
+        <f>A10+7</f>
+        <v>44103</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AML12" s="1"/>
+    </row>
+    <row r="13" ht="63.649999999999999" customHeight="1">
+      <c r="A13" s="5">
+        <f>A11+7</f>
+        <v>44106</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+    </row>
+    <row r="14" ht="99.450000000000003" customHeight="1">
+      <c r="A14" s="5">
+        <f>A12+7</f>
+        <v>44110</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+    </row>
+    <row r="15" ht="68.25" customHeight="1">
+      <c r="A15" s="5">
+        <f>A13+7</f>
+        <v>44113</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+    </row>
+    <row r="16" ht="58.5" customHeight="1">
+      <c r="A16" s="5">
+        <f>A14+7</f>
+        <v>44117</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+    </row>
+    <row r="17" ht="54.75" customHeight="1">
+      <c r="A17" s="5">
+        <f>A15+7</f>
+        <v>44120</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+    </row>
+    <row r="18" ht="55.5" customHeight="1">
+      <c r="A18" s="5">
+        <f>A16+7</f>
+        <v>44124</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+    </row>
+    <row r="19" ht="43.5" customHeight="1">
+      <c r="A19" s="5">
+        <f>A17+7</f>
+        <v>44127</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+    </row>
+    <row r="20" ht="53.25" customHeight="1">
+      <c r="A20" s="5">
+        <f>A18+7</f>
+        <v>44131</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+    </row>
+    <row r="21" ht="39.75" customHeight="1">
+      <c r="A21" s="5">
+        <f>A19+7</f>
+        <v>44134</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+    </row>
+    <row r="22" ht="87.5" customHeight="1">
+      <c r="A22" s="5">
+        <f>A20+7</f>
+        <v>44138</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+    </row>
+    <row r="23" ht="63.649999999999999" customHeight="1">
+      <c r="A23" s="5">
+        <f>A21+7</f>
+        <v>44141</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+    </row>
+    <row r="24" ht="63.649999999999999" customHeight="1">
+      <c r="A24" s="5">
+        <f>A22+7</f>
+        <v>44145</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+    </row>
+    <row r="25" ht="63.649999999999999" customHeight="1">
+      <c r="A25" s="5">
+        <f>A23+7</f>
+        <v>44148</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+    </row>
+    <row r="26" ht="39.75" customHeight="1">
+      <c r="A26" s="5">
+        <f>A24+7</f>
+        <v>44152</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+    </row>
+    <row r="27" ht="39.75" customHeight="1">
+      <c r="A27" s="5">
+        <f>A25+7</f>
+        <v>44155</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8"/>
+    </row>
+    <row r="28" ht="75.549999999999997" customHeight="1">
+      <c r="A28" s="5">
+        <f>A26+7</f>
+        <v>44159</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="8"/>
+    </row>
+    <row r="29" ht="75.549999999999997" customHeight="1">
+      <c r="A29" s="5">
+        <f>A27+7</f>
+        <v>44162</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="8"/>
+      <c r="AA29" s="8"/>
+    </row>
+    <row r="30" ht="111.40000000000001" customHeight="1">
+      <c r="A30" s="5">
+        <f>A28+7</f>
+        <v>44166</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="8"/>
+      <c r="Z30" s="8"/>
+      <c r="AA30" s="8"/>
+    </row>
+    <row r="31" ht="29.399999999999999" customHeight="1">
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="8"/>
+    </row>
+    <row r="32" ht="51.700000000000003" customHeight="1">
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="8"/>
+    </row>
+    <row r="33" ht="51.700000000000003" customHeight="1">
+      <c r="G33" s="7"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="8"/>
+    </row>
+    <row r="34" ht="51.700000000000003" customHeight="1"/>
+    <row r="35" ht="29.399999999999999" customHeight="1"/>
+    <row r="41" ht="15"/>
+    <row r="42" ht="15"/>
+    <row r="43" ht="15"/>
+    <row r="1000" ht="39.75" customHeight="1"/>
+    <row r="1001" ht="15"/>
+    <row r="1002" ht="15"/>
+    <row r="1003" ht="15"/>
+    <row r="1004" ht="15"/>
+    <row r="1005" ht="15"/>
+    <row r="1006" ht="15"/>
+    <row r="1007" ht="15"/>
+    <row r="1008" ht="15"/>
+    <row r="1009" ht="15"/>
+    <row r="1010" ht="15"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr filterMode="0">
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="1" showRowColHeaders="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2381,7 +3637,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -2415,7 +3671,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -2447,10 +3703,10 @@
         <v>43690</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
@@ -2482,10 +3738,10 @@
         <v>43693</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -2517,16 +3773,16 @@
         <v>43697</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="23"/>
@@ -2556,10 +3812,10 @@
         <v>43700</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -2594,13 +3850,13 @@
         <v>33</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="23"/>
@@ -2633,10 +3889,10 @@
         <v>33</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="21"/>
@@ -2670,7 +3926,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -2705,7 +3961,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
@@ -2740,11 +3996,11 @@
         <v>33</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="23"/>
@@ -2777,7 +4033,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -2812,7 +4068,7 @@
         <v>33</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -2847,10 +4103,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
@@ -2881,11 +4137,11 @@
         <v>43732</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="21"/>
@@ -2919,13 +4175,13 @@
         <v>45</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="23"/>
@@ -2958,11 +4214,11 @@
         <v>45</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="23"/>
@@ -2995,13 +4251,13 @@
         <v>45</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="23"/>
@@ -3034,11 +4290,11 @@
         <v>45</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="23"/>
@@ -3071,11 +4327,11 @@
         <v>45</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="23"/>
@@ -3108,10 +4364,10 @@
         <v>45</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="21"/>
@@ -3142,16 +4398,16 @@
         <v>43756</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="23"/>
@@ -3181,13 +4437,13 @@
         <v>43760</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="21"/>
@@ -3218,10 +4474,10 @@
         <v>43763</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -3253,14 +4509,14 @@
         <v>43767</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="23"/>
@@ -3290,16 +4546,16 @@
         <v>43770</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="23"/>
@@ -3329,10 +4585,10 @@
         <v>43774</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -3364,16 +4620,16 @@
         <v>43777</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="23"/>
@@ -3403,10 +4659,10 @@
         <v>43781</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -3438,10 +4694,10 @@
         <v>43784</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -3501,7 +4757,7 @@
         <v>43791</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22"/>
@@ -3542,7 +4798,7 @@
         <v>43798</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22"/>

</xml_diff>